<commit_message>
Updated Configuration log following Flight03
Detailed repairs and component swaps following damage from Flight03.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="146">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -57,39 +57,12 @@
     <t>Accels</t>
   </si>
   <si>
-    <t>As-Built Measures</t>
-  </si>
-  <si>
-    <t>wing spans</t>
-  </si>
-  <si>
-    <t>wing chord</t>
-  </si>
-  <si>
-    <t>control surface length</t>
-  </si>
-  <si>
-    <t>control surface chord</t>
-  </si>
-  <si>
-    <t>spar width</t>
-  </si>
-  <si>
-    <t>spar height</t>
-  </si>
-  <si>
     <t>Sköll</t>
   </si>
   <si>
     <t>Hati</t>
   </si>
   <si>
-    <t>Wing Mass Prop</t>
-  </si>
-  <si>
-    <t>AC Mass Prop</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -303,21 +276,6 @@
     <t>MiniMUTT Class Aircraft - Current Configuration</t>
   </si>
   <si>
-    <t>CB Mass Prop</t>
-  </si>
-  <si>
-    <t>Pitot Location 6DOF</t>
-  </si>
-  <si>
-    <t>Accel Location 6DOF</t>
-  </si>
-  <si>
-    <t>GPS Location 3DOF</t>
-  </si>
-  <si>
-    <t>Camera Location 6DOF</t>
-  </si>
-  <si>
     <t>Motor Mount Base</t>
   </si>
   <si>
@@ -444,9 +402,6 @@
     <t>[Spare WingSet]</t>
   </si>
   <si>
-    <t>Operational 6/15/2015</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -481,6 +436,30 @@
   </si>
   <si>
     <t>Replaced Hemisphere Crescent with Novatel OEMStar</t>
+  </si>
+  <si>
+    <t>Repaired Centerbody nose</t>
+  </si>
+  <si>
+    <t>Replaced Right Wing Servos (004, 005, 006) with (011, 012, 013)</t>
+  </si>
+  <si>
+    <t>Repaired Right Wing Inboard and Outboard Control Surface hinges</t>
+  </si>
+  <si>
+    <t>011</t>
+  </si>
+  <si>
+    <t>012</t>
+  </si>
+  <si>
+    <t>013</t>
+  </si>
+  <si>
+    <t>Repaired Left Outboard Wingtip</t>
+  </si>
+  <si>
+    <t>Operational 7/7/2015</t>
   </si>
 </sst>
 </file>
@@ -720,7 +699,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -755,7 +734,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -964,10 +943,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -977,42 +956,35 @@
     <col min="3" max="3" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.5703125" customWidth="1"/>
     <col min="5" max="5" width="30.140625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="24" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1023,15 +995,12 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>141</v>
-      </c>
-      <c r="G3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>1</v>
@@ -1040,15 +1009,12 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>140</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>3</v>
@@ -1057,100 +1023,62 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>142</v>
-      </c>
-      <c r="G5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>91</v>
-      </c>
-      <c r="G6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G10" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="G11" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="E12" s="1"/>
-      <c r="G12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="G13" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G14" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1158,7 +1086,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1222,7 +1150,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1230,50 +1158,50 @@
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="20"/>
@@ -1288,40 +1216,40 @@
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="19"/>
@@ -1335,39 +1263,39 @@
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -1380,55 +1308,55 @@
     <row r="17" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="20" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="B20" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>48</v>
-      </c>
       <c r="D20" s="20" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D21" s="20"/>
     </row>
@@ -1436,63 +1364,63 @@
     <row r="23" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D25" s="16"/>
     </row>
     <row r="26" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D27" s="20"/>
     </row>
     <row r="28" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B28" s="20" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D28" s="20"/>
     </row>
@@ -1504,15 +1432,15 @@
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1526,10 +1454,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B67" sqref="B67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1541,7 +1469,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1550,42 +1478,42 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="1"/>
@@ -1600,40 +1528,40 @@
     <row r="7" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D10" s="20"/>
       <c r="E10" s="19"/>
@@ -1647,39 +1575,39 @@
     <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="D14" s="9"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="D15" s="4"/>
     </row>
@@ -1692,44 +1620,44 @@
     <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1741,39 +1669,39 @@
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D24" s="9"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D25" s="4"/>
     </row>
@@ -1786,142 +1714,142 @@
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D29" s="16" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>47</v>
-      </c>
       <c r="D30" s="4" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="21" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D31" s="20"/>
     </row>
     <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D35" s="16"/>
     </row>
     <row r="36" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="21" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B36" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D36" s="20"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="21" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B37" s="18" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D37" s="20"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D40" s="4"/>
     </row>
@@ -1933,53 +1861,53 @@
     <row r="42" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="43" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="44" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="9" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C44" s="15" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D44" s="13" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
     </row>
     <row r="45" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="21" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B45" s="21" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="C45" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D45" s="20"/>
     </row>
     <row r="46" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="21" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B46" s="21" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="C46" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D46" s="20"/>
     </row>
@@ -1992,15 +1920,15 @@
     <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2008,7 +1936,7 @@
         <v>42161</v>
       </c>
       <c r="B51" s="25" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2016,7 +1944,7 @@
         <v>42161</v>
       </c>
       <c r="B52" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2024,7 +1952,7 @@
         <v>42164</v>
       </c>
       <c r="B53" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2032,7 +1960,7 @@
         <v>42164</v>
       </c>
       <c r="B54" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2040,7 +1968,7 @@
         <v>42166</v>
       </c>
       <c r="B55" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2048,7 +1976,7 @@
         <v>42167</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="57" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2056,7 +1984,7 @@
         <v>42167</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="58" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2064,7 +1992,7 @@
         <v>42170</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2072,7 +2000,7 @@
         <v>42170</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2080,7 +2008,7 @@
         <v>42179</v>
       </c>
       <c r="B60" s="18" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2088,7 +2016,7 @@
         <v>42179</v>
       </c>
       <c r="B61" s="18" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
     </row>
     <row r="62" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2096,7 +2024,7 @@
         <v>42184</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2104,7 +2032,7 @@
         <v>42184</v>
       </c>
       <c r="B63" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,38 +2040,31 @@
         <v>42184</v>
       </c>
       <c r="B64" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="23"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="23"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="23"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="23"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="23">
+        <v>42191</v>
+      </c>
+      <c r="B65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="23"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="23"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2171,7 +2092,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2203,7 +2124,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2211,7 +2132,7 @@
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2219,55 +2140,55 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7"/>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="1"/>
@@ -2277,28 +2198,28 @@
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D9" s="7"/>
       <c r="E9" s="1"/>
@@ -2308,7 +2229,7 @@
     </row>
     <row r="12" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
@@ -2316,51 +2237,51 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -2369,28 +2290,28 @@
     </row>
     <row r="18" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="1"/>
@@ -2403,15 +2324,15 @@
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2426,10 +2347,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2442,7 +2363,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2450,7 +2371,7 @@
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2458,68 +2379,68 @@
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2528,69 +2449,69 @@
         <v>10</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="D14" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="28" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
@@ -2598,50 +2519,50 @@
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>51</v>
+        <v>141</v>
       </c>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>52</v>
+        <v>142</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>53</v>
+        <v>143</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -2651,78 +2572,78 @@
         <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="D28" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -2730,7 +2651,39 @@
         <v>42170</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23">
+        <v>42184</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="23">
+        <v>42191</v>
+      </c>
+      <c r="B35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="23">
+        <v>42191</v>
+      </c>
+      <c r="B36" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="23">
+        <v>42191</v>
+      </c>
+      <c r="B37" t="s">
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2761,7 +2714,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2793,7 +2746,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2819,15 +2772,15 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B3" s="21">
         <v>95.85</v>
@@ -2835,7 +2788,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="B4" s="21">
         <v>96.45</v>
@@ -2843,46 +2796,46 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B5">
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="B6">
         <v>35</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B7">
         <v>35</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B8">
         <v>35</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mass Property and Configuration Update
Captures Goldy upgrade
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -17,12 +17,12 @@
     <sheet name="WS3" sheetId="8" r:id="rId8"/>
     <sheet name="Components" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="147">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -198,24 +198,6 @@
     <t>Phoenix Edge Lite 75</t>
   </si>
   <si>
-    <t>ADC</t>
-  </si>
-  <si>
-    <t>Left</t>
-  </si>
-  <si>
-    <t>Right</t>
-  </si>
-  <si>
-    <t>PA0060 w/SX8724CWLTDTCT-ND</t>
-  </si>
-  <si>
-    <t>Mounted on Board with Low Pass Filter, Set for Vbatt to D0 (I2C address 100XX01)</t>
-  </si>
-  <si>
-    <t>Mounted on Board with Low Pass Filter, Set for Vbatt to D1 (I2C address 100XX10)</t>
-  </si>
-  <si>
     <t>Power and Propulsion</t>
   </si>
   <si>
@@ -348,9 +330,6 @@
     <t>Installed Goldy SN 006 (removed SN 007)</t>
   </si>
   <si>
-    <t>w/ servo reverser inline</t>
-  </si>
-  <si>
     <t>Added Servo Reverser to L3, adjusted set point to zero</t>
   </si>
   <si>
@@ -396,9 +375,6 @@
     <t>Expert EXRA320</t>
   </si>
   <si>
-    <t>Physically Unmodified</t>
-  </si>
-  <si>
     <t>[Spare WingSet]</t>
   </si>
   <si>
@@ -435,9 +411,6 @@
     <t>Replaced the Hemishere Cresecent with Novatel OEM Star</t>
   </si>
   <si>
-    <t>Replaced Hemisphere Crescent with Novatel OEMStar</t>
-  </si>
-  <si>
     <t>Repaired Centerbody nose</t>
   </si>
   <si>
@@ -460,6 +433,36 @@
   </si>
   <si>
     <t>Operational 7/7/2015</t>
+  </si>
+  <si>
+    <t>Removed Titan III GPS antenna</t>
+  </si>
+  <si>
+    <t>Teensy 3.1</t>
+  </si>
+  <si>
+    <t>Added a Teensy 3.1</t>
+  </si>
+  <si>
+    <t>Removed Novatel OEMStar</t>
+  </si>
+  <si>
+    <t>Changed a whole bunch of wiring</t>
+  </si>
+  <si>
+    <t>Moved servo reverser from wing to centerbody</t>
+  </si>
+  <si>
+    <t>Repaired pitot probe, replaced dynamic pressure and static pressure transducer</t>
+  </si>
+  <si>
+    <t>Replaced Propellor</t>
+  </si>
+  <si>
+    <t>Voltage Divider / Filter</t>
+  </si>
+  <si>
+    <t>Custom. 5V to 3.33V. 35Hz 1st order LPF</t>
   </si>
 </sst>
 </file>
@@ -587,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -638,6 +641,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -946,7 +950,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -960,7 +964,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="26" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="B1" s="26"/>
       <c r="C1" s="26"/>
@@ -995,7 +999,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1009,7 +1013,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1023,18 +1027,18 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1198,10 +1202,10 @@
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="20"/>
@@ -1216,7 +1220,7 @@
     <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="8" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>15</v>
@@ -1230,10 +1234,10 @@
     </row>
     <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>38</v>
@@ -1243,10 +1247,10 @@
     </row>
     <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>39</v>
@@ -1277,7 +1281,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
@@ -1289,7 +1293,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -1308,7 +1312,7 @@
     <row r="17" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>15</v>
@@ -1331,7 +1335,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1345,15 +1349,15 @@
         <v>39</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>39</v>
@@ -1364,7 +1368,7 @@
     <row r="23" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>15</v>
@@ -1378,10 +1382,10 @@
     </row>
     <row r="25" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>38</v>
@@ -1390,10 +1394,10 @@
     </row>
     <row r="26" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>38</v>
@@ -1405,7 +1409,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>38</v>
@@ -1454,10 +1458,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E73"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1478,7 +1482,7 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
@@ -1490,565 +1494,599 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="B4" s="30"/>
+      <c r="C4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>34</v>
-      </c>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="1"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
+      <c r="A6" s="20" t="s">
+        <v>145</v>
+      </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="20"/>
+      <c r="C6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="20" t="s">
+        <v>146</v>
+      </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="5" t="s">
+    <row r="7" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C9" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D9" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C9" s="15" t="s">
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="9"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D10" s="20"/>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C14" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D14" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="9"/>
-    </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>79</v>
+      <c r="A15" s="9" t="s">
+        <v>72</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>133</v>
-      </c>
-      <c r="D15" s="4"/>
+      <c r="C15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
+      <c r="A16" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>125</v>
+      </c>
       <c r="D16" s="4"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="4"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B30" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="9" t="s">
+    <row r="31" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="C35" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="C24" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="16" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="B31" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="C31" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D31" s="20"/>
-    </row>
-    <row r="33" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="s">
-        <v>84</v>
-      </c>
-      <c r="B35" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="C35" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="D35" s="16"/>
-    </row>
-    <row r="36" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="B36" s="18" t="s">
-        <v>85</v>
+      <c r="B36" t="s">
+        <v>59</v>
       </c>
       <c r="C36" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="20"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C37" s="12" t="s">
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="20"/>
+    </row>
+    <row r="38" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="20"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C38" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D38" s="4"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>65</v>
-      </c>
-      <c r="C39" s="12" t="s">
+      <c r="D40" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D39" s="4"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" t="s">
-        <v>65</v>
-      </c>
-      <c r="C40" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="21"/>
-      <c r="C41" s="12"/>
       <c r="D41" s="20"/>
     </row>
-    <row r="42" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="43" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D43" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B44" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C44" s="15" t="s">
+    <row r="42" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D44" s="13" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="B45" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C45" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D45" s="20"/>
-    </row>
-    <row r="46" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="B46" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="C46" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D46" s="20"/>
-    </row>
-    <row r="47" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="21"/>
-      <c r="B47" s="21"/>
-      <c r="C47" s="12"/>
-      <c r="D47" s="20"/>
-    </row>
-    <row r="48" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="5" t="s">
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C46"/>
+      <c r="D46"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24">
+        <v>42161</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" s="18"/>
+      <c r="D47" s="18"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="23">
+        <v>42161</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="23">
+        <v>42164</v>
+      </c>
+      <c r="B49" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="23">
+        <v>42164</v>
+      </c>
+      <c r="B50" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23">
+        <v>42166</v>
+      </c>
+      <c r="B51" t="s">
+        <v>104</v>
+      </c>
+      <c r="C51"/>
+      <c r="D51"/>
+    </row>
+    <row r="52" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23">
+        <v>42167</v>
+      </c>
+      <c r="B52" s="18" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23">
+        <v>42167</v>
+      </c>
+      <c r="B53" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="23">
+        <v>42170</v>
+      </c>
+      <c r="B54" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="C54" s="18"/>
+      <c r="D54" s="18"/>
+    </row>
+    <row r="55" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23">
+        <v>42170</v>
+      </c>
+      <c r="B55" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="24">
-        <v>42161</v>
-      </c>
-      <c r="B51" s="25" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="23">
-        <v>42161</v>
-      </c>
-      <c r="B52" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="23">
-        <v>42164</v>
-      </c>
-      <c r="B53" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="23">
-        <v>42164</v>
-      </c>
-      <c r="B54" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="23">
-        <v>42166</v>
-      </c>
-      <c r="B55" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C55"/>
+      <c r="D55"/>
+    </row>
+    <row r="56" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="23">
-        <v>42167</v>
+        <v>42179</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="23">
-        <v>42167</v>
+        <v>42179</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="23">
-        <v>42170</v>
+        <v>42184</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+        <v>123</v>
+      </c>
+      <c r="C58" s="18"/>
+      <c r="D58" s="18"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="23">
-        <v>42170</v>
+        <v>42184</v>
       </c>
       <c r="B59" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="23">
-        <v>42179</v>
-      </c>
-      <c r="B60" s="18" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42184</v>
+      </c>
+      <c r="B60" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="23">
-        <v>42179</v>
-      </c>
-      <c r="B61" s="18" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
+        <v>42191</v>
+      </c>
+      <c r="B61" t="s">
+        <v>129</v>
+      </c>
+      <c r="C61"/>
+      <c r="D61"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="23">
-        <v>42184</v>
+        <v>42217</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="C62" s="18"/>
+      <c r="D62" s="18"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="23">
-        <v>42184</v>
+        <v>42217</v>
       </c>
       <c r="B63" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="23">
-        <v>42184</v>
+        <v>42217</v>
       </c>
       <c r="B64" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="23">
-        <v>42191</v>
+        <v>42217</v>
       </c>
       <c r="B65" t="s">
-        <v>138</v>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="23">
+        <v>42217</v>
+      </c>
+      <c r="B66" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="23">
+        <v>42217</v>
+      </c>
+      <c r="B67" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="23">
+        <v>42219</v>
+      </c>
+      <c r="B68" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2056,15 +2094,6 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="23"/>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="23"/>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2077,26 +2106,475 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A47" sqref="A47:B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" width="24.7109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="18"/>
+    <col min="4" max="4" width="36.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="27" t="s">
         <v>20</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="30"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="30"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>138</v>
+      </c>
+      <c r="B5" s="21"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="B6" s="21"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>116</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="20"/>
+    </row>
+    <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="19"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="19"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="B11" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="11"/>
+      <c r="D15" s="9"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="12"/>
+      <c r="D16" s="20"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="11"/>
+      <c r="D20" s="9"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B25" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="20"/>
+    </row>
+    <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C31" s="15"/>
+      <c r="D31" s="16"/>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B32" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="20"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="C33" s="12"/>
+      <c r="D33" s="20"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>56</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C34" s="12"/>
+      <c r="D34" s="20"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="12"/>
+      <c r="D35" s="20"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="12"/>
+      <c r="D36" s="20"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="21"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="20"/>
+    </row>
+    <row r="38" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="15"/>
+      <c r="D40" s="13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="20"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B42" s="21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="12"/>
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="20"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="5" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="24"/>
+      <c r="B47" s="25"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="23"/>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" s="23"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" s="23"/>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" s="23"/>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" s="23"/>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23"/>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" s="23"/>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" s="23"/>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" s="23"/>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" s="23"/>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" s="23"/>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" s="23"/>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" s="23"/>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" s="23"/>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="23"/>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" s="23"/>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" s="23"/>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="23"/>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="23"/>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="23"/>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="23"/>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="23"/>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2154,7 +2632,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>26</v>
@@ -2167,7 +2645,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>26</v>
@@ -2176,13 +2654,13 @@
         <v>39</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>26</v>
@@ -2216,7 +2694,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>38</v>
@@ -2251,7 +2729,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B14" s="7" t="s">
         <v>26</v>
@@ -2263,7 +2741,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>26</v>
@@ -2275,7 +2753,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>26</v>
@@ -2308,7 +2786,7 @@
         <v>48</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>39</v>
@@ -2347,10 +2825,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2393,7 +2871,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>49</v>
@@ -2405,7 +2883,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>49</v>
@@ -2413,13 +2891,11 @@
       <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="21" t="s">
-        <v>108</v>
-      </c>
+      <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>49</v>
@@ -2429,20 +2905,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>122</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>123</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="20" t="s">
-        <v>124</v>
-      </c>
-    </row>
+    <row r="7" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
@@ -2502,7 +2965,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>38</v>
@@ -2533,36 +2996,36 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -2625,7 +3088,7 @@
         <v>48</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>39</v>
@@ -2651,7 +3114,7 @@
         <v>42170</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2659,7 +3122,7 @@
         <v>42184</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -2667,7 +3130,7 @@
         <v>42191</v>
       </c>
       <c r="B35" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -2675,7 +3138,7 @@
         <v>42191</v>
       </c>
       <c r="B36" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -2683,7 +3146,15 @@
         <v>42191</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="23">
+        <v>42217</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -2698,18 +3169,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" style="18" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -2720,9 +3192,266 @@
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
     </row>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="11"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="12"/>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="11"/>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="11"/>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C28" s="11"/>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="23"/>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2772,15 +3501,15 @@
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2" t="s">
         <v>114</v>
-      </c>
-      <c r="B2" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B3" s="21">
         <v>95.85</v>
@@ -2788,7 +3517,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="18" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B4" s="21">
         <v>96.45</v>
@@ -2796,46 +3525,46 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="18" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B5">
         <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="18" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B6">
         <v>35</v>
       </c>
       <c r="C6" s="18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B7">
         <v>35</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="18" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B8">
         <v>35</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Configuration Updates following Skoll Flight 6
Configuration and Mass Property Update following flight 6. These are
applicable for flight 7, 8, and 9.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="149">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -463,6 +463,12 @@
   </si>
   <si>
     <t>Custom. 5V to 3.33V. 35Hz 1st order LPF</t>
+  </si>
+  <si>
+    <t>Repaired wing attaches</t>
+  </si>
+  <si>
+    <t>Replaced 7 of 8 servos</t>
   </si>
 </sst>
 </file>
@@ -629,6 +635,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -641,7 +648,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -949,7 +955,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
@@ -963,13 +969,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1153,12 +1159,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
@@ -1458,10 +1464,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1472,12 +1478,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1498,11 +1504,11 @@
       <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="D4" s="30"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -2090,10 +2096,52 @@
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="23"/>
+      <c r="A69" s="23">
+        <v>42225</v>
+      </c>
+      <c r="B69" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="23"/>
+      <c r="A70" s="23">
+        <v>42225</v>
+      </c>
+      <c r="B70" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="23">
+        <v>42225</v>
+      </c>
+      <c r="B71" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="23"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="23"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="23"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="23"/>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="23"/>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="23"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="23"/>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2122,12 +2170,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2148,9 +2196,9 @@
       <c r="A4" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="30"/>
+      <c r="B4" s="26"/>
       <c r="C4" s="12"/>
-      <c r="D4" s="30"/>
+      <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
@@ -2601,20 +2649,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2706,12 +2754,12 @@
       <c r="E10" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
@@ -2840,20 +2888,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -2973,12 +3021,12 @@
       <c r="D14" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -3185,20 +3233,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
@@ -3305,12 +3353,12 @@
       <c r="D14" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B17" s="29"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
     </row>
     <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
@@ -3474,12 +3522,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Removed Skoll, added Hati
Skoll is no longer in configuration control. Hati is now in
configuration control. WS3 fabrication has started.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -15,14 +15,13 @@
     <sheet name="WS1" sheetId="6" r:id="rId6"/>
     <sheet name="WS2" sheetId="7" r:id="rId7"/>
     <sheet name="WS3" sheetId="8" r:id="rId8"/>
-    <sheet name="Components" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="157">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -252,9 +251,6 @@
     <t>Body Flap - Right</t>
   </si>
   <si>
-    <t>Planning</t>
-  </si>
-  <si>
     <t>MiniMUTT Class Aircraft - Current Configuration</t>
   </si>
   <si>
@@ -345,30 +341,6 @@
     <t>Painted Orange on wing tops</t>
   </si>
   <si>
-    <t>Winglets</t>
-  </si>
-  <si>
-    <t>SN 001</t>
-  </si>
-  <si>
-    <t>SN 002</t>
-  </si>
-  <si>
-    <t>SN 003</t>
-  </si>
-  <si>
-    <t>SN 004</t>
-  </si>
-  <si>
-    <t>SN 005</t>
-  </si>
-  <si>
-    <t>SN 006</t>
-  </si>
-  <si>
-    <t>Mass</t>
-  </si>
-  <si>
     <t>Servo Reverser</t>
   </si>
   <si>
@@ -381,15 +353,9 @@
     <t>Storage</t>
   </si>
   <si>
-    <t>In Assembly</t>
-  </si>
-  <si>
     <t>Added Voltage Dividers on Accelerometer signals</t>
   </si>
   <si>
-    <t>Approx</t>
-  </si>
-  <si>
     <t>Replaced Servo 007 with 009, 008 with 010.</t>
   </si>
   <si>
@@ -432,9 +398,6 @@
     <t>Repaired Left Outboard Wingtip</t>
   </si>
   <si>
-    <t>Operational 7/7/2015</t>
-  </si>
-  <si>
     <t>Removed Titan III GPS antenna</t>
   </si>
   <si>
@@ -469,6 +432,66 @@
   </si>
   <si>
     <t>Replaced 7 of 8 servos</t>
+  </si>
+  <si>
+    <t>014</t>
+  </si>
+  <si>
+    <t>015</t>
+  </si>
+  <si>
+    <t>Modified to be shorter</t>
+  </si>
+  <si>
+    <t>016</t>
+  </si>
+  <si>
+    <t>017</t>
+  </si>
+  <si>
+    <t>018</t>
+  </si>
+  <si>
+    <t>019</t>
+  </si>
+  <si>
+    <t>020</t>
+  </si>
+  <si>
+    <t>021</t>
+  </si>
+  <si>
+    <t>022</t>
+  </si>
+  <si>
+    <t>023</t>
+  </si>
+  <si>
+    <t>Sköll Stiff Wings</t>
+  </si>
+  <si>
+    <t>Requires Repair</t>
+  </si>
+  <si>
+    <t>In Test</t>
+  </si>
+  <si>
+    <t>In Work</t>
+  </si>
+  <si>
+    <t>Hati Flexible Wings</t>
+  </si>
+  <si>
+    <t>Hati Spar Wings</t>
+  </si>
+  <si>
+    <t>Left Wing Spar is Broken at Wing attach</t>
+  </si>
+  <si>
+    <t>Wing folded during last flight, unkown damage</t>
+  </si>
+  <si>
+    <t>Left Wing is severly damaged, no longer tracking changes</t>
   </si>
 </sst>
 </file>
@@ -955,8 +978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,7 +993,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="24" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -1005,7 +1028,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,7 +1042,7 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1033,18 +1056,18 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>119</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1076,14 +1099,20 @@
       <c r="A14" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="B14" s="18" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B15" s="21" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>17</v>
       </c>
@@ -1091,30 +1120,45 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B19" s="18" t="s">
+        <v>148</v>
+      </c>
+      <c r="C19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B25" s="1"/>
     </row>
   </sheetData>
@@ -1208,10 +1252,10 @@
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="21" t="s">
         <v>91</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>92</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="20"/>
@@ -1243,7 +1287,7 @@
         <v>74</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>38</v>
@@ -1256,7 +1300,7 @@
         <v>75</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>39</v>
@@ -1318,7 +1362,7 @@
     <row r="17" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>15</v>
@@ -1341,7 +1385,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1355,15 +1399,15 @@
         <v>39</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B21" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>39</v>
@@ -1388,10 +1432,10 @@
     </row>
     <row r="25" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>38</v>
@@ -1400,10 +1444,10 @@
     </row>
     <row r="26" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>38</v>
@@ -1415,7 +1459,7 @@
         <v>54</v>
       </c>
       <c r="B27" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C27" s="6" t="s">
         <v>38</v>
@@ -1466,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="A72" sqref="A72"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1488,7 +1532,7 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
@@ -1512,7 +1556,7 @@
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
@@ -1523,23 +1567,23 @@
     </row>
     <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>39</v>
@@ -1567,7 +1611,7 @@
         <v>74</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C10" s="15" t="s">
         <v>38</v>
@@ -1580,7 +1624,7 @@
         <v>75</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>39</v>
@@ -1616,7 +1660,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D15" s="9"/>
     </row>
@@ -1628,7 +1672,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -1686,7 +1730,7 @@
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>15</v>
@@ -1709,7 +1753,7 @@
         <v>39</v>
       </c>
       <c r="D25" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1723,15 +1767,15 @@
         <v>39</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>89</v>
       </c>
       <c r="C27" s="12" t="s">
         <v>40</v>
@@ -1755,10 +1799,10 @@
     </row>
     <row r="31" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>78</v>
-      </c>
-      <c r="B31" s="9" t="s">
-        <v>79</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>39</v>
@@ -1767,10 +1811,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C32" s="12" t="s">
         <v>39</v>
@@ -1847,7 +1891,7 @@
     </row>
     <row r="40" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>63</v>
@@ -1856,12 +1900,12 @@
         <v>38</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>63</v>
@@ -1873,10 +1917,10 @@
     </row>
     <row r="42" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>85</v>
-      </c>
-      <c r="B42" s="21" t="s">
-        <v>86</v>
       </c>
       <c r="C42" s="12" t="s">
         <v>38</v>
@@ -1892,7 +1936,7 @@
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:4" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1910,7 +1954,7 @@
         <v>42161</v>
       </c>
       <c r="B47" s="25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C47" s="18"/>
       <c r="D47" s="18"/>
@@ -1920,7 +1964,7 @@
         <v>42161</v>
       </c>
       <c r="B48" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1928,7 +1972,7 @@
         <v>42164</v>
       </c>
       <c r="B49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1936,7 +1980,7 @@
         <v>42164</v>
       </c>
       <c r="B50" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="51" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1944,7 +1988,7 @@
         <v>42166</v>
       </c>
       <c r="B51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C51"/>
       <c r="D51"/>
@@ -1954,7 +1998,7 @@
         <v>42167</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="53" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1962,7 +2006,7 @@
         <v>42167</v>
       </c>
       <c r="B53" s="18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1970,7 +2014,7 @@
         <v>42170</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -1980,7 +2024,7 @@
         <v>42170</v>
       </c>
       <c r="B55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C55"/>
       <c r="D55"/>
@@ -1990,7 +2034,7 @@
         <v>42179</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -1998,7 +2042,7 @@
         <v>42179</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2006,7 +2050,7 @@
         <v>42184</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>123</v>
+        <v>112</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -2016,7 +2060,7 @@
         <v>42184</v>
       </c>
       <c r="B59" t="s">
-        <v>122</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2024,7 +2068,7 @@
         <v>42184</v>
       </c>
       <c r="B60" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2032,7 +2076,7 @@
         <v>42191</v>
       </c>
       <c r="B61" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
       <c r="C61"/>
       <c r="D61"/>
@@ -2042,7 +2086,7 @@
         <v>42217</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -2052,7 +2096,7 @@
         <v>42217</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2060,7 +2104,7 @@
         <v>42217</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2068,7 +2112,7 @@
         <v>42217</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2076,7 +2120,7 @@
         <v>42217</v>
       </c>
       <c r="B66" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2084,7 +2128,7 @@
         <v>42217</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2092,7 +2136,7 @@
         <v>42219</v>
       </c>
       <c r="B68" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2100,7 +2144,7 @@
         <v>42225</v>
       </c>
       <c r="B69" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2108,7 +2152,7 @@
         <v>42225</v>
       </c>
       <c r="B70" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2116,7 +2160,7 @@
         <v>42225</v>
       </c>
       <c r="B71" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2156,8 +2200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:B47"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2180,7 +2224,7 @@
     <row r="2" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>15</v>
@@ -2197,38 +2241,48 @@
         <v>9</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="12"/>
+      <c r="C4" s="12" t="s">
+        <v>52</v>
+      </c>
       <c r="D4" s="26"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="B5" s="21"/>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D5" s="20"/>
       <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B6" s="21"/>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="D6" s="20" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="20"/>
+        <v>107</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="20" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2251,9 +2305,11 @@
         <v>74</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C10" s="15"/>
+        <v>78</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="D10" s="9"/>
       <c r="E10" s="19"/>
     </row>
@@ -2262,9 +2318,11 @@
         <v>75</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C11" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2295,7 +2353,9 @@
       <c r="B15" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="11"/>
+      <c r="C15" s="11" t="s">
+        <v>146</v>
+      </c>
       <c r="D15" s="9"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2305,7 +2365,9 @@
       <c r="B16" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C16" s="12"/>
+      <c r="C16" s="12" t="s">
+        <v>147</v>
+      </c>
       <c r="D16" s="20"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -2336,7 +2398,9 @@
       <c r="B20" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="11"/>
+      <c r="C20" s="11" t="s">
+        <v>121</v>
+      </c>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -2346,7 +2410,9 @@
       <c r="B21" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>122</v>
+      </c>
       <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -2358,7 +2424,7 @@
     <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="24" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>15</v>
@@ -2377,9 +2443,11 @@
       <c r="B25" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="15"/>
+      <c r="C25" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="D25" s="16" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -2389,19 +2457,23 @@
       <c r="B26" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="12"/>
+      <c r="C26" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="D26" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B27" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="B27" s="21" t="s">
-        <v>89</v>
-      </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="D27" s="20"/>
     </row>
     <row r="29" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2421,22 +2493,26 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B31" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C31" s="15"/>
+      <c r="C31" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="D31" s="16"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B32" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C32" s="12"/>
+        <v>78</v>
+      </c>
+      <c r="C32" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D32" s="20"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -2446,7 +2522,9 @@
       <c r="B33" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="12" t="s">
+        <v>39</v>
+      </c>
       <c r="D33" s="20"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -2456,7 +2534,9 @@
       <c r="B34" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="D34" s="20"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -2466,7 +2546,9 @@
       <c r="B35" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>40</v>
+      </c>
       <c r="D35" s="20"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -2476,7 +2558,9 @@
       <c r="B36" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>42</v>
+      </c>
       <c r="D36" s="20"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -2501,34 +2585,40 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B40" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="C40" s="15"/>
+      <c r="C40" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="D40" s="13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B41" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C41" s="12"/>
+      <c r="C41" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D41" s="20"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="B42" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="B42" s="21" t="s">
-        <v>86</v>
-      </c>
-      <c r="C42" s="12"/>
+      <c r="C42" s="12" t="s">
+        <v>38</v>
+      </c>
       <c r="D42" s="20"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -2540,7 +2630,7 @@
     <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2742,7 +2832,7 @@
         <v>48</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>38</v>
@@ -2834,7 +2924,7 @@
         <v>48</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>39</v>
@@ -2873,10 +2963,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D38"/>
+  <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2925,7 +3015,7 @@
         <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -2937,7 +3027,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D5" s="21"/>
     </row>
@@ -2949,7 +3039,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>40</v>
+        <v>123</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -3013,7 +3103,7 @@
         <v>48</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>38</v>
@@ -3050,7 +3140,7 @@
         <v>49</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>132</v>
+        <v>39</v>
       </c>
       <c r="D19" s="7"/>
     </row>
@@ -3062,7 +3152,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3073,7 +3163,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -3136,7 +3226,7 @@
         <v>48</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C28" s="11" t="s">
         <v>39</v>
@@ -3162,7 +3252,7 @@
         <v>42170</v>
       </c>
       <c r="B33" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:2" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -3170,7 +3260,7 @@
         <v>42184</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3178,7 +3268,7 @@
         <v>42191</v>
       </c>
       <c r="B35" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3186,7 +3276,7 @@
         <v>42191</v>
       </c>
       <c r="B36" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3194,7 +3284,7 @@
         <v>42191</v>
       </c>
       <c r="B37" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3202,7 +3292,12 @@
         <v>42217</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>142</v>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -3219,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3269,7 +3364,9 @@
       <c r="B4" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C4" s="11"/>
+      <c r="C4" s="11" t="s">
+        <v>140</v>
+      </c>
       <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3279,7 +3376,9 @@
       <c r="B5" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="12" t="s">
+        <v>141</v>
+      </c>
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3289,7 +3388,9 @@
       <c r="B6" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="12" t="s">
+        <v>142</v>
+      </c>
       <c r="D6" s="20"/>
     </row>
     <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3314,7 +3415,9 @@
       <c r="B10" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="11"/>
+      <c r="C10" s="11" t="s">
+        <v>52</v>
+      </c>
       <c r="D10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3324,7 +3427,9 @@
       <c r="B11" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="12"/>
+      <c r="C11" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="D11" s="20"/>
     </row>
     <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3347,9 +3452,11 @@
         <v>48</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C14" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>40</v>
+      </c>
       <c r="D14" s="7"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -3381,7 +3488,9 @@
       <c r="B19" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C19" s="11"/>
+      <c r="C19" s="11" t="s">
+        <v>143</v>
+      </c>
       <c r="D19" s="7"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3391,7 +3500,9 @@
       <c r="B20" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="12" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
@@ -3400,7 +3511,9 @@
       <c r="B21" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="12" t="s">
+        <v>145</v>
+      </c>
       <c r="D21" s="20"/>
     </row>
     <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3425,7 +3538,9 @@
       <c r="B24" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="C24" s="11"/>
+      <c r="C24" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="D24" s="7"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3435,7 +3550,9 @@
       <c r="B25" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="12"/>
+      <c r="C25" s="12" t="s">
+        <v>114</v>
+      </c>
       <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3458,9 +3575,11 @@
         <v>48</v>
       </c>
       <c r="B28" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="C28" s="11"/>
+        <v>78</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>42</v>
+      </c>
       <c r="D28" s="7"/>
     </row>
     <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -3535,87 +3654,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>108</v>
-      </c>
-      <c r="B3" s="21">
-        <v>95.85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="21">
-        <v>96.45</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B5">
-        <v>35</v>
-      </c>
-      <c r="C5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>111</v>
-      </c>
-      <c r="B6">
-        <v>35</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>112</v>
-      </c>
-      <c r="B7">
-        <v>35</v>
-      </c>
-      <c r="C7" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>113</v>
-      </c>
-      <c r="B8">
-        <v>35</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>121</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Config and Mass Tracking
Hati with WS2 and WS3 are under configuration control. Still need Servo
serial numbers added to the configuration of WS3.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="164">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -347,9 +347,6 @@
     <t>Expert EXRA320</t>
   </si>
   <si>
-    <t>[Spare WingSet]</t>
-  </si>
-  <si>
     <t>Storage</t>
   </si>
   <si>
@@ -473,18 +470,12 @@
     <t>Requires Repair</t>
   </si>
   <si>
-    <t>In Test</t>
-  </si>
-  <si>
     <t>In Work</t>
   </si>
   <si>
     <t>Hati Flexible Wings</t>
   </si>
   <si>
-    <t>Hati Spar Wings</t>
-  </si>
-  <si>
     <t>Left Wing Spar is Broken at Wing attach</t>
   </si>
   <si>
@@ -492,6 +483,36 @@
   </si>
   <si>
     <t>Left Wing is severly damaged, no longer tracking changes</t>
+  </si>
+  <si>
+    <t>Hati Stiff Wings</t>
+  </si>
+  <si>
+    <t>9/29/2015</t>
+  </si>
+  <si>
+    <t>Mass Property Testing with CB2</t>
+  </si>
+  <si>
+    <t>Wing is severly damaged</t>
+  </si>
+  <si>
+    <t>Mass Property Tested with WS2</t>
+  </si>
+  <si>
+    <t>Mass Property Tested with WS3</t>
+  </si>
+  <si>
+    <t>Replaced Pitot probe</t>
+  </si>
+  <si>
+    <t>9/24/2015</t>
+  </si>
+  <si>
+    <t>9/1/2015</t>
+  </si>
+  <si>
+    <t>9/30/2015</t>
   </si>
 </sst>
 </file>
@@ -978,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1028,7 +1049,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,32 +1063,26 @@
         <v>4</v>
       </c>
       <c r="E4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
-        <v>150</v>
-      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>3</v>
       </c>
       <c r="D6" s="22" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1128,7 +1143,7 @@
         <v>19</v>
       </c>
       <c r="C18" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1136,10 +1151,10 @@
         <v>4</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C19" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1147,7 +1162,7 @@
         <v>5</v>
       </c>
       <c r="B20" s="21" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1155,7 +1170,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="21" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1176,7 +1191,7 @@
     <hyperlink ref="C3" location="CB0!A1" display="CB0"/>
     <hyperlink ref="D3" location="WS0!A1" display="WS0"/>
     <hyperlink ref="C4" location="'CB1'!A1" display="CB1"/>
-    <hyperlink ref="C5" location="'CB2'!A1" display="CB2"/>
+    <hyperlink ref="C6" location="'CB2'!A1" display="CB2"/>
     <hyperlink ref="D4" location="'WS1'!A1" display="WS1"/>
     <hyperlink ref="D5" location="'WS2'!A1" display="WS2"/>
     <hyperlink ref="D6" location="'WS3'!A1" display="WS3"/>
@@ -1510,8 +1525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1556,7 +1571,7 @@
     </row>
     <row r="5" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
@@ -1567,14 +1582,14 @@
     </row>
     <row r="6" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" s="19"/>
     </row>
@@ -1660,7 +1675,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D15" s="9"/>
     </row>
@@ -1672,7 +1687,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D16" s="4"/>
     </row>
@@ -2014,7 +2029,7 @@
         <v>42170</v>
       </c>
       <c r="B54" s="18" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C54" s="18"/>
       <c r="D54" s="18"/>
@@ -2034,7 +2049,7 @@
         <v>42179</v>
       </c>
       <c r="B56" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2042,7 +2057,7 @@
         <v>42179</v>
       </c>
       <c r="B57" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -2050,7 +2065,7 @@
         <v>42184</v>
       </c>
       <c r="B58" s="18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C58" s="18"/>
       <c r="D58" s="18"/>
@@ -2060,7 +2075,7 @@
         <v>42184</v>
       </c>
       <c r="B59" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -2068,7 +2083,7 @@
         <v>42184</v>
       </c>
       <c r="B60" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.25">
@@ -2076,7 +2091,7 @@
         <v>42191</v>
       </c>
       <c r="B61" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C61"/>
       <c r="D61"/>
@@ -2086,7 +2101,7 @@
         <v>42217</v>
       </c>
       <c r="B62" s="18" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="18"/>
       <c r="D62" s="18"/>
@@ -2096,7 +2111,7 @@
         <v>42217</v>
       </c>
       <c r="B63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -2104,7 +2119,7 @@
         <v>42217</v>
       </c>
       <c r="B64" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2112,7 +2127,7 @@
         <v>42217</v>
       </c>
       <c r="B65" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2120,7 +2135,7 @@
         <v>42217</v>
       </c>
       <c r="B66" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2128,7 +2143,7 @@
         <v>42217</v>
       </c>
       <c r="B67" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2136,7 +2151,7 @@
         <v>42219</v>
       </c>
       <c r="B68" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2144,7 +2159,7 @@
         <v>42225</v>
       </c>
       <c r="B69" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2167,7 @@
         <v>42225</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2160,7 +2175,7 @@
         <v>42225</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2200,8 +2215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2248,7 +2263,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="21"/>
       <c r="C5" s="12" t="s">
@@ -2259,14 +2274,14 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B6" s="21"/>
       <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E6" s="19"/>
     </row>
@@ -2281,7 +2296,7 @@
         <v>40</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2354,7 +2369,7 @@
         <v>49</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D15" s="9"/>
     </row>
@@ -2366,7 +2381,7 @@
         <v>49</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D16" s="20"/>
     </row>
@@ -2399,7 +2414,7 @@
         <v>50</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D20" s="9"/>
     </row>
@@ -2411,7 +2426,7 @@
         <v>50</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="20"/>
     </row>
@@ -2472,7 +2487,7 @@
         <v>88</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D27" s="20"/>
     </row>
@@ -2642,58 +2657,72 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="24"/>
-      <c r="B47" s="25"/>
+      <c r="A47" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B47" s="25" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="23"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="23"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="23"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="23"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
@@ -2724,10 +2753,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2949,6 +2978,11 @@
       </c>
       <c r="B23" s="5" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>
@@ -2965,7 +2999,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
@@ -3039,7 +3073,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D6" s="4"/>
     </row>
@@ -3152,7 +3186,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3163,7 +3197,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D21" s="4"/>
     </row>
@@ -3260,7 +3294,7 @@
         <v>42184</v>
       </c>
       <c r="B34" s="18" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -3268,7 +3302,7 @@
         <v>42191</v>
       </c>
       <c r="B35" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -3276,7 +3310,7 @@
         <v>42191</v>
       </c>
       <c r="B36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -3284,7 +3318,7 @@
         <v>42191</v>
       </c>
       <c r="B37" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -3292,12 +3326,12 @@
         <v>42217</v>
       </c>
       <c r="B38" s="18" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3314,8 +3348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3365,7 +3399,7 @@
         <v>49</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D4" s="7"/>
     </row>
@@ -3377,7 +3411,7 @@
         <v>49</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D5" s="21"/>
     </row>
@@ -3389,7 +3423,7 @@
         <v>49</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D6" s="20"/>
     </row>
@@ -3489,7 +3523,7 @@
         <v>49</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D19" s="7"/>
     </row>
@@ -3501,7 +3535,7 @@
         <v>49</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,7 +3546,7 @@
         <v>49</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D21" s="20"/>
     </row>
@@ -3539,7 +3573,7 @@
         <v>50</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D24" s="7"/>
     </row>
@@ -3551,7 +3585,7 @@
         <v>50</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D25" s="20"/>
     </row>
@@ -3596,22 +3630,27 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="23"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>162</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="23"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="23"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="23"/>
     </row>
   </sheetData>
@@ -3626,18 +3665,19 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" customWidth="1"/>
-    <col min="4" max="4" width="37.5703125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="37.5703125" style="18" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
@@ -3648,9 +3688,283 @@
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
+    <row r="2" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30"/>
+    </row>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="11"/>
+      <c r="D4" s="7"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="21"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="20"/>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B11" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="D11" s="20"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="13" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="7"/>
+    </row>
+    <row r="17" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="11"/>
+      <c r="D19" s="7"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="12"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="12"/>
+      <c r="D21" s="20"/>
+    </row>
+    <row r="22" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="D24" s="7"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="D25" s="20"/>
+    </row>
+    <row r="26" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="7"/>
+    </row>
+    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
+        <v>155</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="23"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="23"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="23"/>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="23"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="23"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Config Tracking and Mass Properties Tracking
Updated for Motor swap following abort prior to FLT05. Replaced GPS with
Ublox M8N.
</commit_message>
<xml_diff>
--- a/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
+++ b/Design/CAD/mAEWing1 - Configuration Tracking.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9405" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="771" uniqueCount="178">
   <si>
     <t>MiniMUTT Class Aircraft</t>
   </si>
@@ -548,6 +548,15 @@
   </si>
   <si>
     <t>025</t>
+  </si>
+  <si>
+    <t>Swapped ESC to SN003</t>
+  </si>
+  <si>
+    <t>Swapped Motor to SN003</t>
+  </si>
+  <si>
+    <t>Changed GPS from Ublox 7p to Ublox M8N</t>
   </si>
 </sst>
 </file>
@@ -1283,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3155,8 +3164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E70"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3476,7 +3485,7 @@
         <v>55</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D33" s="20"/>
     </row>
@@ -3488,7 +3497,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D34" s="20"/>
     </row>
@@ -3603,14 +3612,28 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="23"/>
+      <c r="A48" s="23">
+        <v>42634</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="23"/>
-      <c r="B49" s="21"/>
+      <c r="A49" s="23">
+        <v>42647</v>
+      </c>
+      <c r="B49" s="21" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="23"/>
+      <c r="A50" s="23">
+        <v>42647</v>
+      </c>
+      <c r="B50" s="21" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>

</xml_diff>